<commit_message>
Security Monitoring  assessment excel + question/guidance standardization
</commit_message>
<xml_diff>
--- a/Supporting Resources/v1.5/MarkDown/Draft/SAMM_Assessment_Toolbox_v1.5.1.xlsx
+++ b/Supporting Resources/v1.5/MarkDown/Draft/SAMM_Assessment_Toolbox_v1.5.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoRo/LocalProgramming/Repositories/SAMM/Supporting Resources/v1.5/MarkDown/Draft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ACE810-0EB6-5E42-A806-5CEBF423A63F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF84A0F-26D8-3649-8F07-8BE30386ADA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10300" yWindow="-23540" windowWidth="32540" windowHeight="23080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="677">
   <si>
     <t>Are stakeholders aware of options for additional tools to protect software while running in operations?</t>
   </si>
@@ -1592,12 +1592,6 @@
     <t>Lifecycle Security Culture</t>
   </si>
   <si>
-    <t>___?</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Lifecycle Security Design</t>
   </si>
   <si>
@@ -2007,6 +2001,126 @@
   </si>
   <si>
     <t>Release gates are enhanced with penetration test results.</t>
+  </si>
+  <si>
+    <t>Does your organization gather information about new vulnerability issues?</t>
+  </si>
+  <si>
+    <t>Are vulnerability issues filtered to dedicated project, used hardware and software stacks?</t>
+  </si>
+  <si>
+    <t>Are there project teams after final (serial) release responsible for these issues?</t>
+  </si>
+  <si>
+    <t>Every team or part of it has to maintain their project after the release (including security concerns).</t>
+  </si>
+  <si>
+    <t>Developers consider 3rd party libraries in their development and testing lifecycle.</t>
+  </si>
+  <si>
+    <t>A newly found vulnerability is immediately transmitted to all affected teams.</t>
+  </si>
+  <si>
+    <t>Every project records all used hardware and software, including 3rd party.</t>
+  </si>
+  <si>
+    <t>Every team knows whom to contact about newly found vulnerability issues.</t>
+  </si>
+  <si>
+    <t>All contracts with subcontractors require them to report security flaws they discover.</t>
+  </si>
+  <si>
+    <t>Feeds about vulnerability issues are monitored.</t>
+  </si>
+  <si>
+    <t>The company regularly checks for new sources for vulnerabilities.</t>
+  </si>
+  <si>
+    <t>Is your penetration test continuously developed?</t>
+  </si>
+  <si>
+    <t>Do you assure that penetration tests are executed for every released hardware/software combination?</t>
+  </si>
+  <si>
+    <t>Does your company collect and archive all results of these penetration tests?</t>
+  </si>
+  <si>
+    <t>Penetration tests are well documented.</t>
+  </si>
+  <si>
+    <t>Found issues are reported and documented.</t>
+  </si>
+  <si>
+    <t>The software and hardware combinations that are vulnerable to a specific attack are documented immediately.</t>
+  </si>
+  <si>
+    <t>Penetration tests are evaluated regularly.</t>
+  </si>
+  <si>
+    <t>Penetration testers have the goal to find new vulnerabilities.</t>
+  </si>
+  <si>
+    <t>New externally found vulnerabilities are added to the penetration tests.</t>
+  </si>
+  <si>
+    <t>Penetration tests are executed for every project.</t>
+  </si>
+  <si>
+    <t>Every possible HW/SW combination is documented.</t>
+  </si>
+  <si>
+    <t>Every new rollout generates new penetration tests.</t>
+  </si>
+  <si>
+    <t>Temporarily security establishing workarounds do not impede safety or functionality of the product, which must be ensured by tests.</t>
+  </si>
+  <si>
+    <t>Software and hardware are prioritized depending on if it's in the field or not.</t>
+  </si>
+  <si>
+    <t>Does your company know how to contact the end users of your devices?</t>
+  </si>
+  <si>
+    <t>Does your company have a process which defines the propagation of security vulnerabilities to your customers?</t>
+  </si>
+  <si>
+    <t>Does your company have a process which defines the propagation of security updates to end users?</t>
+  </si>
+  <si>
+    <t>Do your project teams provide a security degradation guidance model?</t>
+  </si>
+  <si>
+    <t>The company has guidelines how to define a security update process.</t>
+  </si>
+  <si>
+    <t>Software updates reach the customer mostly unnoticed.</t>
+  </si>
+  <si>
+    <t>An update channel is established.</t>
+  </si>
+  <si>
+    <t>Project teams are required to implement software in their projects that enable updates and degradation.</t>
+  </si>
+  <si>
+    <t>Customers are made aware of all possible risks and actions in case of a security issue.</t>
+  </si>
+  <si>
+    <t>A database with hardware and software in the field is maintained.</t>
+  </si>
+  <si>
+    <t>The company has guidelines how to handle found security issues.</t>
+  </si>
+  <si>
+    <t>The company defines the handling of found security issues in the contract with its customers.</t>
+  </si>
+  <si>
+    <t>Customers with affected software and/or hardware can be identified.</t>
+  </si>
+  <si>
+    <t>The company has records of all customers.</t>
+  </si>
+  <si>
+    <t>Customer can be contacted sufficiently, within a specific time frame and future save.</t>
   </si>
 </sst>
 </file>
@@ -2331,7 +2445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="133">
+  <borders count="137">
     <border>
       <left/>
       <right/>
@@ -3931,6 +4045,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3942,7 +4104,7 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="579">
+  <cellXfs count="587">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5593,6 +5755,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="132" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="102" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="14" borderId="104" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="127" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="134" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="133" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="119" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="136" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -6593,7 +6779,7 @@
                   <c:v>1.1499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.75</c:v>
+                  <c:v>0.67500000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8069,7 +8255,7 @@
                   <c:v>1.1499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.75</c:v>
+                  <c:v>0.67500000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12979,7 +13165,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.75</c:v>
+                  <c:v>0.67500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.5</c:v>
@@ -17521,10 +17707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z642"/>
+  <dimension ref="A1:Z660"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B447" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E467" sqref="E467"/>
+    <sheetView tabSelected="1" topLeftCell="B618" zoomScale="128" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D634" sqref="D634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -21845,10 +22031,10 @@
     </row>
     <row r="137" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B137" s="305" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C137" s="334" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D137" s="335"/>
       <c r="E137" s="5" t="s">
@@ -21893,7 +22079,7 @@
         <v>370</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -21924,7 +22110,7 @@
         <v>370</v>
       </c>
       <c r="D139" s="291" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E139" s="288"/>
       <c r="F139" s="25"/>
@@ -21955,7 +22141,7 @@
         <v>370</v>
       </c>
       <c r="D140" s="19" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E140" s="30"/>
       <c r="F140" s="25"/>
@@ -22010,7 +22196,7 @@
     <row r="142" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B142" s="306"/>
       <c r="C142" s="332" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D142" s="333"/>
       <c r="E142" s="22" t="s">
@@ -22049,7 +22235,7 @@
         <v>370</v>
       </c>
       <c r="D143" s="290" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E143" s="289"/>
       <c r="F143" s="24"/>
@@ -22080,7 +22266,7 @@
         <v>370</v>
       </c>
       <c r="D144" s="291" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E144" s="288"/>
       <c r="F144" s="25"/>
@@ -22111,7 +22297,7 @@
         <v>370</v>
       </c>
       <c r="D145" s="291" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E145" s="288"/>
       <c r="F145" s="25"/>
@@ -22166,7 +22352,7 @@
     <row r="147" spans="2:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B147" s="387"/>
       <c r="C147" s="353" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D147" s="354"/>
       <c r="E147" s="282" t="s">
@@ -22205,7 +22391,7 @@
         <v>370</v>
       </c>
       <c r="D148" s="20" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E148" s="279"/>
       <c r="F148" s="280"/>
@@ -22236,7 +22422,7 @@
         <v>370</v>
       </c>
       <c r="D149" s="291" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="E149" s="288"/>
       <c r="F149" s="280"/>
@@ -22267,7 +22453,7 @@
         <v>370</v>
       </c>
       <c r="D150" s="291" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E150" s="288"/>
       <c r="F150" s="280"/>
@@ -22348,10 +22534,10 @@
     </row>
     <row r="153" spans="2:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B153" s="305" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C153" s="334" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D153" s="335"/>
       <c r="E153" s="5" t="s">
@@ -22393,7 +22579,7 @@
         <v>370</v>
       </c>
       <c r="D154" s="20" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E154" s="29"/>
       <c r="F154" s="24"/>
@@ -22424,7 +22610,7 @@
         <v>370</v>
       </c>
       <c r="D155" s="291" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E155" s="288"/>
       <c r="F155" s="25"/>
@@ -22479,7 +22665,7 @@
     <row r="157" spans="2:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B157" s="306"/>
       <c r="C157" s="332" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D157" s="333"/>
       <c r="E157" s="22" t="s">
@@ -22518,7 +22704,7 @@
         <v>370</v>
       </c>
       <c r="D158" s="20" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E158" s="29"/>
       <c r="F158" s="24"/>
@@ -22549,7 +22735,7 @@
         <v>370</v>
       </c>
       <c r="D159" s="291" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E159" s="288"/>
       <c r="F159" s="25"/>
@@ -22604,7 +22790,7 @@
     <row r="161" spans="2:26" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B161" s="387"/>
       <c r="C161" s="294" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D161" s="295"/>
       <c r="E161" s="285" t="s">
@@ -22643,7 +22829,7 @@
         <v>370</v>
       </c>
       <c r="D162" s="20" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E162" s="279"/>
       <c r="F162" s="280"/>
@@ -22674,7 +22860,7 @@
         <v>370</v>
       </c>
       <c r="D163" s="291" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E163" s="288"/>
       <c r="F163" s="280"/>
@@ -22755,10 +22941,10 @@
     </row>
     <row r="166" spans="2:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B166" s="305" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C166" s="334" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D166" s="335"/>
       <c r="E166" s="5" t="s">
@@ -22800,7 +22986,7 @@
         <v>370</v>
       </c>
       <c r="D167" s="20" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E167" s="29"/>
       <c r="F167" s="24"/>
@@ -22855,7 +23041,7 @@
     <row r="169" spans="2:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B169" s="306"/>
       <c r="C169" s="332" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D169" s="333"/>
       <c r="E169" s="22" t="s">
@@ -22894,7 +23080,7 @@
         <v>370</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E170" s="29"/>
       <c r="F170" s="24"/>
@@ -22925,7 +23111,7 @@
         <v>370</v>
       </c>
       <c r="D171" s="291" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E171" s="288"/>
       <c r="F171" s="25"/>
@@ -22980,7 +23166,7 @@
     <row r="173" spans="2:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B173" s="387"/>
       <c r="C173" s="294" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D173" s="295"/>
       <c r="E173" s="285" t="s">
@@ -23019,7 +23205,7 @@
         <v>370</v>
       </c>
       <c r="D174" s="20" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E174" s="279"/>
       <c r="F174" s="280"/>
@@ -23050,7 +23236,7 @@
         <v>370</v>
       </c>
       <c r="D175" s="291" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E175" s="288"/>
       <c r="F175" s="280"/>
@@ -26387,7 +26573,7 @@
     <row r="278" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A278"/>
       <c r="B278" s="314" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C278" s="315"/>
       <c r="D278" s="316"/>
@@ -26423,10 +26609,10 @@
     <row r="279" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A279"/>
       <c r="B279" s="323" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C279" s="400" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D279" s="401"/>
       <c r="E279" s="5" t="s">
@@ -26472,7 +26658,7 @@
         <v>370</v>
       </c>
       <c r="D280" s="20" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E280" s="29"/>
       <c r="F280" s="24"/>
@@ -26504,7 +26690,7 @@
         <v>370</v>
       </c>
       <c r="D281" s="291" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E281" s="288"/>
       <c r="F281" s="25"/>
@@ -26536,7 +26722,7 @@
         <v>370</v>
       </c>
       <c r="D282" s="291" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E282" s="288"/>
       <c r="F282" s="280"/>
@@ -26568,7 +26754,7 @@
         <v>370</v>
       </c>
       <c r="D283" s="19" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E283" s="30"/>
       <c r="F283" s="25"/>
@@ -26625,7 +26811,7 @@
       <c r="A285"/>
       <c r="B285" s="324"/>
       <c r="C285" s="403" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D285" s="404"/>
       <c r="E285" s="22" t="s">
@@ -26665,7 +26851,7 @@
         <v>370</v>
       </c>
       <c r="D286" s="20" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E286" s="29"/>
       <c r="F286" s="24"/>
@@ -26697,7 +26883,7 @@
         <v>370</v>
       </c>
       <c r="D287" s="291" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E287" s="288"/>
       <c r="F287" s="25"/>
@@ -26729,7 +26915,7 @@
         <v>370</v>
       </c>
       <c r="D288" s="291" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E288" s="288"/>
       <c r="F288" s="280"/>
@@ -26761,7 +26947,7 @@
         <v>370</v>
       </c>
       <c r="D289" s="19" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E289" s="30"/>
       <c r="F289" s="25"/>
@@ -26845,10 +27031,10 @@
     <row r="292" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A292"/>
       <c r="B292" s="323" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C292" s="334" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D292" s="335"/>
       <c r="E292" s="5" t="s">
@@ -26891,7 +27077,7 @@
         <v>370</v>
       </c>
       <c r="D293" s="290" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E293" s="289"/>
       <c r="F293" s="24"/>
@@ -26923,7 +27109,7 @@
         <v>370</v>
       </c>
       <c r="D294" s="291" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E294" s="288"/>
       <c r="F294" s="25"/>
@@ -26955,7 +27141,7 @@
         <v>370</v>
       </c>
       <c r="D295" s="291" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E295" s="288"/>
       <c r="F295" s="25"/>
@@ -27012,7 +27198,7 @@
       <c r="A297"/>
       <c r="B297" s="324"/>
       <c r="C297" s="551" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D297" s="552"/>
       <c r="E297" s="549" t="s">
@@ -27052,7 +27238,7 @@
         <v>370</v>
       </c>
       <c r="D298" s="290" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E298" s="289"/>
       <c r="F298" s="24"/>
@@ -27084,7 +27270,7 @@
         <v>370</v>
       </c>
       <c r="D299" s="291" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E299" s="288"/>
       <c r="F299" s="25"/>
@@ -27116,7 +27302,7 @@
         <v>370</v>
       </c>
       <c r="D300" s="291" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E300" s="288"/>
       <c r="F300" s="25"/>
@@ -27173,7 +27359,7 @@
       <c r="A302"/>
       <c r="B302" s="399"/>
       <c r="C302" s="553" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D302" s="554"/>
       <c r="E302" s="549" t="s">
@@ -27213,7 +27399,7 @@
         <v>370</v>
       </c>
       <c r="D303" s="290" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E303" s="289"/>
       <c r="F303" s="24"/>
@@ -27245,7 +27431,7 @@
         <v>370</v>
       </c>
       <c r="D304" s="291" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E304" s="288"/>
       <c r="F304" s="25"/>
@@ -27277,7 +27463,7 @@
         <v>370</v>
       </c>
       <c r="D305" s="291" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E305" s="288"/>
       <c r="F305" s="25"/>
@@ -27334,7 +27520,7 @@
       <c r="A307"/>
       <c r="B307" s="399"/>
       <c r="C307" s="553" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D307" s="554"/>
       <c r="E307" s="549" t="s">
@@ -27374,7 +27560,7 @@
         <v>370</v>
       </c>
       <c r="D308" s="290" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E308" s="289"/>
       <c r="F308" s="24"/>
@@ -27406,7 +27592,7 @@
         <v>370</v>
       </c>
       <c r="D309" s="291" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E309" s="288"/>
       <c r="F309" s="25"/>
@@ -27438,7 +27624,7 @@
         <v>370</v>
       </c>
       <c r="D310" s="291" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E310" s="288"/>
       <c r="F310" s="25"/>
@@ -27470,7 +27656,7 @@
         <v>370</v>
       </c>
       <c r="D311" s="291" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E311" s="288"/>
       <c r="F311" s="25"/>
@@ -27554,10 +27740,10 @@
     <row r="314" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A314"/>
       <c r="B314" s="323" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C314" s="559" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D314" s="560"/>
       <c r="E314" s="555" t="s">
@@ -27600,7 +27786,7 @@
         <v>370</v>
       </c>
       <c r="D315" s="562" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E315" s="556"/>
       <c r="F315" s="24"/>
@@ -27632,7 +27818,7 @@
         <v>370</v>
       </c>
       <c r="D316" s="291" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E316" s="288"/>
       <c r="F316" s="25"/>
@@ -27689,7 +27875,7 @@
       <c r="A318"/>
       <c r="B318" s="324"/>
       <c r="C318" s="551" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D318" s="552"/>
       <c r="E318" s="549" t="s">
@@ -27729,7 +27915,7 @@
         <v>370</v>
       </c>
       <c r="D319" s="562" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E319" s="556"/>
       <c r="F319" s="24"/>
@@ -27761,7 +27947,7 @@
         <v>370</v>
       </c>
       <c r="D320" s="291" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E320" s="288"/>
       <c r="F320" s="25"/>
@@ -27793,7 +27979,7 @@
         <v>370</v>
       </c>
       <c r="D321" s="291" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E321" s="288"/>
       <c r="F321" s="25"/>
@@ -27825,7 +28011,7 @@
         <v>370</v>
       </c>
       <c r="D322" s="291" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E322" s="288"/>
       <c r="F322" s="25"/>
@@ -27882,7 +28068,7 @@
       <c r="A324"/>
       <c r="B324" s="399"/>
       <c r="C324" s="294" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D324" s="565"/>
       <c r="E324" s="558" t="s">
@@ -27922,7 +28108,7 @@
         <v>370</v>
       </c>
       <c r="D325" s="291" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E325" s="288"/>
       <c r="F325" s="280"/>
@@ -27954,7 +28140,7 @@
         <v>370</v>
       </c>
       <c r="D326" s="291" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="E326" s="288"/>
       <c r="F326" s="280"/>
@@ -28011,7 +28197,7 @@
       <c r="A328"/>
       <c r="B328" s="399"/>
       <c r="C328" s="294" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D328" s="565"/>
       <c r="E328" s="558" t="s">
@@ -28051,7 +28237,7 @@
         <v>370</v>
       </c>
       <c r="D329" s="291" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="E329" s="288"/>
       <c r="F329" s="280"/>
@@ -28083,7 +28269,7 @@
         <v>370</v>
       </c>
       <c r="D330" s="291" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E330" s="288"/>
       <c r="F330" s="280"/>
@@ -28115,7 +28301,7 @@
         <v>370</v>
       </c>
       <c r="D331" s="291" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E331" s="288"/>
       <c r="F331" s="280"/>
@@ -28147,7 +28333,7 @@
         <v>370</v>
       </c>
       <c r="D332" s="291" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E332" s="288"/>
       <c r="F332" s="280"/>
@@ -31430,7 +31616,7 @@
     <row r="433" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A433"/>
       <c r="B433" s="308" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C433" s="309"/>
       <c r="D433" s="310"/>
@@ -31466,10 +31652,10 @@
     <row r="434" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A434"/>
       <c r="B434" s="348" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C434" s="400" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D434" s="401"/>
       <c r="E434" s="5" t="s">
@@ -31515,7 +31701,7 @@
         <v>370</v>
       </c>
       <c r="D435" s="20" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E435" s="29"/>
       <c r="F435" s="24"/>
@@ -31547,7 +31733,7 @@
         <v>370</v>
       </c>
       <c r="D436" s="291" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E436" s="288"/>
       <c r="F436" s="25"/>
@@ -31604,7 +31790,7 @@
       <c r="A438"/>
       <c r="B438" s="349"/>
       <c r="C438" s="403" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D438" s="404"/>
       <c r="E438" s="22" t="s">
@@ -31644,7 +31830,7 @@
         <v>370</v>
       </c>
       <c r="D439" s="20" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="E439" s="29"/>
       <c r="F439" s="24"/>
@@ -31676,7 +31862,7 @@
         <v>370</v>
       </c>
       <c r="D440" s="291" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E440" s="288"/>
       <c r="F440" s="280"/>
@@ -31708,7 +31894,7 @@
         <v>370</v>
       </c>
       <c r="D441" s="291" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E441" s="288"/>
       <c r="F441" s="25"/>
@@ -31765,7 +31951,7 @@
       <c r="A443"/>
       <c r="B443" s="349"/>
       <c r="C443" s="403" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D443" s="404"/>
       <c r="E443" s="282" t="s">
@@ -31805,7 +31991,7 @@
         <v>370</v>
       </c>
       <c r="D444" s="562" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E444" s="556"/>
       <c r="F444" s="24"/>
@@ -31837,7 +32023,7 @@
         <v>370</v>
       </c>
       <c r="D445" s="291" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E445" s="288"/>
       <c r="F445" s="280"/>
@@ -31869,7 +32055,7 @@
         <v>370</v>
       </c>
       <c r="D446" s="291" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E446" s="288"/>
       <c r="F446" s="25"/>
@@ -31926,7 +32112,7 @@
       <c r="A448"/>
       <c r="B448" s="571"/>
       <c r="C448" s="575" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D448" s="576"/>
       <c r="E448" s="574" t="s">
@@ -31966,7 +32152,7 @@
         <v>370</v>
       </c>
       <c r="D449" s="291" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E449" s="288"/>
       <c r="F449" s="280"/>
@@ -31998,7 +32184,7 @@
         <v>370</v>
       </c>
       <c r="D450" s="291" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E450" s="288"/>
       <c r="F450" s="280"/>
@@ -32030,7 +32216,7 @@
         <v>370</v>
       </c>
       <c r="D451" s="291" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E451" s="288"/>
       <c r="F451" s="280"/>
@@ -32114,10 +32300,10 @@
     <row r="454" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A454"/>
       <c r="B454" s="348" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C454" s="334" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D454" s="335"/>
       <c r="E454" s="5" t="s">
@@ -32160,7 +32346,7 @@
         <v>370</v>
       </c>
       <c r="D455" s="20" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E455" s="29"/>
       <c r="F455" s="24"/>
@@ -32192,7 +32378,7 @@
         <v>370</v>
       </c>
       <c r="D456" s="291" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E456" s="288"/>
       <c r="F456" s="25"/>
@@ -32224,7 +32410,7 @@
         <v>370</v>
       </c>
       <c r="D457" s="291" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E457" s="288"/>
       <c r="F457" s="25"/>
@@ -32256,7 +32442,7 @@
         <v>370</v>
       </c>
       <c r="D458" s="291" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E458" s="288"/>
       <c r="F458" s="280"/>
@@ -32288,7 +32474,7 @@
         <v>370</v>
       </c>
       <c r="D459" s="291" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E459" s="288"/>
       <c r="F459" s="280"/>
@@ -32320,7 +32506,7 @@
         <v>370</v>
       </c>
       <c r="D460" s="291" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E460" s="288"/>
       <c r="F460" s="280"/>
@@ -32377,7 +32563,7 @@
       <c r="A462"/>
       <c r="B462" s="349"/>
       <c r="C462" s="332" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D462" s="333"/>
       <c r="E462" s="22" t="s">
@@ -32417,7 +32603,7 @@
         <v>370</v>
       </c>
       <c r="D463" s="20" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E463" s="29"/>
       <c r="F463" s="24"/>
@@ -32449,7 +32635,7 @@
         <v>370</v>
       </c>
       <c r="D464" s="291" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E464" s="288"/>
       <c r="F464" s="25"/>
@@ -32481,7 +32667,7 @@
         <v>370</v>
       </c>
       <c r="D465" s="291" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E465" s="288"/>
       <c r="F465" s="280"/>
@@ -32513,7 +32699,7 @@
         <v>370</v>
       </c>
       <c r="D466" s="291" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="E466" s="288"/>
       <c r="F466" s="280"/>
@@ -32545,7 +32731,7 @@
         <v>370</v>
       </c>
       <c r="D467" s="291" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="E467" s="288"/>
       <c r="F467" s="280"/>
@@ -32577,7 +32763,7 @@
         <v>370</v>
       </c>
       <c r="D468" s="291" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E468" s="288"/>
       <c r="F468" s="280"/>
@@ -32609,7 +32795,7 @@
         <v>370</v>
       </c>
       <c r="D469" s="291" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E469" s="288"/>
       <c r="F469" s="280"/>
@@ -32641,7 +32827,7 @@
         <v>370</v>
       </c>
       <c r="D470" s="291" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="E470" s="288"/>
       <c r="F470" s="280"/>
@@ -32673,7 +32859,7 @@
         <v>370</v>
       </c>
       <c r="D471" s="291" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E471" s="288"/>
       <c r="F471" s="25"/>
@@ -32730,7 +32916,7 @@
       <c r="A473"/>
       <c r="B473" s="349"/>
       <c r="C473" s="572" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D473" s="573"/>
       <c r="E473" s="282" t="s">
@@ -32770,7 +32956,7 @@
         <v>370</v>
       </c>
       <c r="D474" s="20" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E474" s="29"/>
       <c r="F474" s="24"/>
@@ -32802,7 +32988,7 @@
         <v>370</v>
       </c>
       <c r="D475" s="291" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="E475" s="288"/>
       <c r="F475" s="280"/>
@@ -32834,7 +33020,7 @@
         <v>370</v>
       </c>
       <c r="D476" s="291" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="E476" s="288"/>
       <c r="F476" s="25"/>
@@ -32918,10 +33104,10 @@
     <row r="479" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A479"/>
       <c r="B479" s="348" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C479" s="577" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D479" s="578"/>
       <c r="E479" s="22" t="s">
@@ -32964,7 +33150,7 @@
         <v>370</v>
       </c>
       <c r="D480" s="547" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E480" s="29"/>
       <c r="F480" s="24"/>
@@ -32996,7 +33182,7 @@
         <v>370</v>
       </c>
       <c r="D481" s="291" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E481" s="288"/>
       <c r="F481" s="280"/>
@@ -33028,7 +33214,7 @@
         <v>370</v>
       </c>
       <c r="D482" s="291" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E482" s="288"/>
       <c r="F482" s="280"/>
@@ -33060,7 +33246,7 @@
         <v>370</v>
       </c>
       <c r="D483" s="291" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E483" s="288"/>
       <c r="F483" s="25"/>
@@ -33092,7 +33278,7 @@
         <v>370</v>
       </c>
       <c r="D484" s="291" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E484" s="288"/>
       <c r="F484" s="25"/>
@@ -33149,7 +33335,7 @@
       <c r="A486"/>
       <c r="B486" s="349"/>
       <c r="C486" s="572" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D486" s="573"/>
       <c r="E486" s="22" t="s">
@@ -33189,7 +33375,7 @@
         <v>370</v>
       </c>
       <c r="D487" s="547" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E487" s="29"/>
       <c r="F487" s="24"/>
@@ -33221,7 +33407,7 @@
         <v>370</v>
       </c>
       <c r="D488" s="291" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E488" s="288"/>
       <c r="F488" s="280"/>
@@ -33253,7 +33439,7 @@
         <v>370</v>
       </c>
       <c r="D489" s="291" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E489" s="288"/>
       <c r="F489" s="280"/>
@@ -33285,7 +33471,7 @@
         <v>370</v>
       </c>
       <c r="D490" s="19" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E490" s="288"/>
       <c r="F490" s="280"/>
@@ -33317,7 +33503,7 @@
         <v>370</v>
       </c>
       <c r="D491" s="291" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E491" s="288"/>
       <c r="F491" s="25"/>
@@ -33349,7 +33535,7 @@
         <v>370</v>
       </c>
       <c r="D492" s="291" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E492" s="288"/>
       <c r="F492" s="25"/>
@@ -37051,7 +37237,7 @@
     </row>
     <row r="606" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B606" s="342" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C606" s="343"/>
       <c r="D606" s="344"/>
@@ -37070,10 +37256,10 @@
     </row>
     <row r="607" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B607" s="336" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C607" s="400" t="s">
-        <v>500</v>
+        <v>637</v>
       </c>
       <c r="D607" s="401"/>
       <c r="E607" s="5" t="s">
@@ -37087,13 +37273,13 @@
         <v>0.2</v>
       </c>
       <c r="H607" s="104">
-        <f>IFERROR(AVERAGE(G607,G612),0)</f>
-        <v>0.2</v>
+        <f>IFERROR(AVERAGE(G607,G613,G617),0)</f>
+        <v>0.20000000000000004</v>
       </c>
       <c r="I607" s="326"/>
       <c r="J607" s="345">
-        <f>SUM(H607,H618,H631)</f>
-        <v>0.75</v>
+        <f>SUM(H607,H622,H640)</f>
+        <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="608" spans="1:26" x14ac:dyDescent="0.15">
@@ -37102,7 +37288,7 @@
         <v>370</v>
       </c>
       <c r="D608" s="20" t="s">
-        <v>501</v>
+        <v>644</v>
       </c>
       <c r="E608" s="29"/>
       <c r="F608" s="24"/>
@@ -37116,10 +37302,10 @@
       <c r="C609" s="210" t="s">
         <v>370</v>
       </c>
-      <c r="D609" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E609" s="30"/>
+      <c r="D609" s="291" t="s">
+        <v>645</v>
+      </c>
+      <c r="E609" s="288"/>
       <c r="F609" s="25"/>
       <c r="G609" s="25"/>
       <c r="H609" s="116"/>
@@ -37127,79 +37313,79 @@
       <c r="J609" s="346"/>
     </row>
     <row r="610" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B610" s="337"/>
+      <c r="B610" s="579"/>
       <c r="C610" s="210" t="s">
         <v>370</v>
       </c>
-      <c r="D610" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E610" s="30"/>
-      <c r="F610" s="25"/>
-      <c r="G610" s="25"/>
-      <c r="H610" s="116"/>
+      <c r="D610" s="291" t="s">
+        <v>646</v>
+      </c>
+      <c r="E610" s="288"/>
+      <c r="F610" s="280"/>
+      <c r="G610" s="280"/>
+      <c r="H610" s="281"/>
       <c r="I610" s="327"/>
-      <c r="J610" s="346"/>
-    </row>
-    <row r="611" spans="2:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="J610" s="580"/>
+    </row>
+    <row r="611" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B611" s="337"/>
-      <c r="C611" s="212"/>
-      <c r="D611" s="21"/>
-      <c r="E611" s="31"/>
-      <c r="F611" s="26"/>
-      <c r="G611" s="26"/>
-      <c r="H611" s="117"/>
-      <c r="I611" s="328"/>
-      <c r="J611" s="347"/>
-    </row>
-    <row r="612" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="C611" s="210" t="s">
+        <v>370</v>
+      </c>
+      <c r="D611" s="291" t="s">
+        <v>647</v>
+      </c>
+      <c r="E611" s="288"/>
+      <c r="F611" s="25"/>
+      <c r="G611" s="25"/>
+      <c r="H611" s="116"/>
+      <c r="I611" s="327"/>
+      <c r="J611" s="346"/>
+    </row>
+    <row r="612" spans="2:10" ht="13" x14ac:dyDescent="0.15">
       <c r="B612" s="337"/>
-      <c r="C612" s="403" t="s">
-        <v>500</v>
-      </c>
-      <c r="D612" s="404"/>
-      <c r="E612" s="22" t="s">
-        <v>490</v>
-      </c>
-      <c r="F612" s="18">
-        <v>21</v>
-      </c>
-      <c r="G612" s="18">
-        <f>IFERROR(VLOOKUP(E612,AnswerCTBL,2,FALSE),0)</f>
-        <v>0.2</v>
-      </c>
-      <c r="H612" s="104"/>
-      <c r="I612" s="326"/>
-      <c r="J612" s="11"/>
+      <c r="C612" s="212"/>
+      <c r="D612" s="21"/>
+      <c r="E612" s="31"/>
+      <c r="F612" s="26"/>
+      <c r="G612" s="26"/>
+      <c r="H612" s="117"/>
+      <c r="I612" s="328"/>
+      <c r="J612" s="347"/>
     </row>
     <row r="613" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B613" s="337"/>
-      <c r="C613" s="209" t="s">
-        <v>370</v>
-      </c>
-      <c r="D613" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E613" s="29"/>
-      <c r="F613" s="24"/>
-      <c r="G613" s="24"/>
-      <c r="H613" s="118"/>
-      <c r="I613" s="327"/>
+      <c r="C613" s="403" t="s">
+        <v>638</v>
+      </c>
+      <c r="D613" s="404"/>
+      <c r="E613" s="22" t="s">
+        <v>490</v>
+      </c>
+      <c r="F613" s="18">
+        <v>21</v>
+      </c>
+      <c r="G613" s="18">
+        <f>IFERROR(VLOOKUP(E613,AnswerCTBL,2,FALSE),0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H613" s="104"/>
+      <c r="I613" s="582"/>
       <c r="J613" s="11"/>
     </row>
     <row r="614" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B614" s="337"/>
-      <c r="C614" s="210" t="s">
+      <c r="C614" s="209" t="s">
         <v>370</v>
       </c>
       <c r="D614" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E614" s="30"/>
-      <c r="F614" s="25"/>
-      <c r="G614" s="25"/>
-      <c r="H614" s="116"/>
-      <c r="I614" s="327"/>
+        <v>643</v>
+      </c>
+      <c r="E614" s="29"/>
+      <c r="F614" s="24"/>
+      <c r="G614" s="24"/>
+      <c r="H614" s="118"/>
+      <c r="I614" s="397"/>
       <c r="J614" s="11"/>
     </row>
     <row r="615" spans="2:10" x14ac:dyDescent="0.15">
@@ -37207,422 +37393,688 @@
       <c r="C615" s="210" t="s">
         <v>370</v>
       </c>
-      <c r="D615" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E615" s="30"/>
+      <c r="D615" s="291" t="s">
+        <v>642</v>
+      </c>
+      <c r="E615" s="288"/>
       <c r="F615" s="25"/>
       <c r="G615" s="25"/>
       <c r="H615" s="116"/>
-      <c r="I615" s="327"/>
+      <c r="I615" s="397"/>
       <c r="J615" s="11"/>
     </row>
     <row r="616" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B616" s="337"/>
-      <c r="C616" s="212"/>
-      <c r="D616" s="21"/>
-      <c r="E616" s="31"/>
-      <c r="F616" s="26"/>
-      <c r="G616" s="26"/>
-      <c r="H616" s="117"/>
-      <c r="I616" s="328"/>
-      <c r="J616" s="11"/>
+      <c r="B616" s="579"/>
+      <c r="C616" s="278"/>
+      <c r="D616" s="19"/>
+      <c r="E616" s="279"/>
+      <c r="F616" s="280"/>
+      <c r="G616" s="280"/>
+      <c r="H616" s="281"/>
+      <c r="I616" s="570"/>
+      <c r="J616" s="277"/>
     </row>
     <row r="617" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B617" s="339"/>
-      <c r="C617" s="340"/>
-      <c r="D617" s="340"/>
-      <c r="E617" s="340"/>
-      <c r="F617" s="340"/>
-      <c r="G617" s="340"/>
-      <c r="H617" s="340"/>
-      <c r="I617" s="341"/>
-      <c r="J617" s="11"/>
+      <c r="B617" s="579"/>
+      <c r="C617" s="294" t="s">
+        <v>639</v>
+      </c>
+      <c r="D617" s="295"/>
+      <c r="E617" s="282" t="s">
+        <v>490</v>
+      </c>
+      <c r="F617" s="283">
+        <v>22</v>
+      </c>
+      <c r="G617" s="283">
+        <f>IFERROR(VLOOKUP(E617,AnswerCTBL,2,FALSE),0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H617" s="284"/>
+      <c r="I617" s="585"/>
+      <c r="J617" s="277"/>
     </row>
     <row r="618" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B618" s="336" t="s">
-        <v>506</v>
-      </c>
-      <c r="C618" s="334" t="s">
-        <v>500</v>
-      </c>
-      <c r="D618" s="335"/>
-      <c r="E618" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="F618" s="18">
-        <v>22</v>
-      </c>
-      <c r="G618" s="18">
-        <f>IFERROR(VLOOKUP(E618,AnswerCTBL,2,FALSE),0)</f>
-        <v>0.2</v>
-      </c>
-      <c r="H618" s="104">
-        <f>IFERROR(AVERAGE(G618,G625),0)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I618" s="326"/>
-      <c r="J618" s="11"/>
+      <c r="B618" s="579"/>
+      <c r="C618" s="278" t="s">
+        <v>370</v>
+      </c>
+      <c r="D618" s="19" t="s">
+        <v>640</v>
+      </c>
+      <c r="E618" s="279"/>
+      <c r="F618" s="280"/>
+      <c r="G618" s="280"/>
+      <c r="H618" s="281"/>
+      <c r="I618" s="397"/>
+      <c r="J618" s="277"/>
     </row>
     <row r="619" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B619" s="337"/>
-      <c r="C619" s="209" t="s">
+      <c r="B619" s="579"/>
+      <c r="C619" s="210" t="s">
         <v>370</v>
       </c>
-      <c r="D619" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E619" s="29"/>
-      <c r="F619" s="24"/>
-      <c r="G619" s="24"/>
-      <c r="H619" s="118"/>
-      <c r="I619" s="327"/>
-      <c r="J619" s="11"/>
+      <c r="D619" s="291" t="s">
+        <v>641</v>
+      </c>
+      <c r="E619" s="288"/>
+      <c r="F619" s="280"/>
+      <c r="G619" s="280"/>
+      <c r="H619" s="281"/>
+      <c r="I619" s="397"/>
+      <c r="J619" s="277"/>
     </row>
     <row r="620" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B620" s="337"/>
-      <c r="C620" s="210" t="s">
-        <v>370</v>
-      </c>
-      <c r="D620" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E620" s="30"/>
-      <c r="F620" s="25"/>
-      <c r="G620" s="25"/>
-      <c r="H620" s="116"/>
-      <c r="I620" s="327"/>
+      <c r="C620" s="212"/>
+      <c r="D620" s="21"/>
+      <c r="E620" s="31"/>
+      <c r="F620" s="26"/>
+      <c r="G620" s="26"/>
+      <c r="H620" s="117"/>
+      <c r="I620" s="569"/>
       <c r="J620" s="11"/>
     </row>
     <row r="621" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B621" s="337"/>
-      <c r="C621" s="210" t="s">
-        <v>370</v>
-      </c>
-      <c r="D621" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E621" s="30"/>
-      <c r="F621" s="25"/>
-      <c r="G621" s="25"/>
-      <c r="H621" s="116"/>
-      <c r="I621" s="327"/>
+      <c r="B621" s="339"/>
+      <c r="C621" s="340"/>
+      <c r="D621" s="340"/>
+      <c r="E621" s="340"/>
+      <c r="F621" s="340"/>
+      <c r="G621" s="340"/>
+      <c r="H621" s="340"/>
+      <c r="I621" s="341"/>
       <c r="J621" s="11"/>
     </row>
     <row r="622" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B622" s="337"/>
-      <c r="C622" s="210" t="s">
-        <v>370</v>
-      </c>
-      <c r="D622" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E622" s="30"/>
-      <c r="F622" s="25"/>
-      <c r="G622" s="25"/>
-      <c r="H622" s="116"/>
-      <c r="I622" s="327"/>
+      <c r="B622" s="336" t="s">
+        <v>504</v>
+      </c>
+      <c r="C622" s="334" t="s">
+        <v>648</v>
+      </c>
+      <c r="D622" s="335"/>
+      <c r="E622" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="F622" s="18">
+        <v>23</v>
+      </c>
+      <c r="G622" s="18">
+        <f>IFERROR(VLOOKUP(E622,AnswerCTBL,2,FALSE),0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H622" s="104">
+        <f>IFERROR(AVERAGE(G622,G627,G633),0)</f>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="I622" s="326"/>
       <c r="J622" s="11"/>
     </row>
     <row r="623" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B623" s="337"/>
-      <c r="C623" s="210" t="s">
+      <c r="C623" s="209" t="s">
         <v>370</v>
       </c>
       <c r="D623" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E623" s="30"/>
-      <c r="F623" s="25"/>
-      <c r="G623" s="25"/>
-      <c r="H623" s="116"/>
+        <v>654</v>
+      </c>
+      <c r="E623" s="29"/>
+      <c r="F623" s="24"/>
+      <c r="G623" s="24"/>
+      <c r="H623" s="118"/>
       <c r="I623" s="327"/>
       <c r="J623" s="11"/>
     </row>
     <row r="624" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B624" s="337"/>
-      <c r="C624" s="212"/>
-      <c r="D624" s="21"/>
-      <c r="E624" s="31"/>
-      <c r="F624" s="26"/>
-      <c r="G624" s="26"/>
-      <c r="H624" s="117"/>
-      <c r="I624" s="328"/>
+      <c r="C624" s="210" t="s">
+        <v>370</v>
+      </c>
+      <c r="D624" s="291" t="s">
+        <v>655</v>
+      </c>
+      <c r="E624" s="288"/>
+      <c r="F624" s="25"/>
+      <c r="G624" s="25"/>
+      <c r="H624" s="116"/>
+      <c r="I624" s="327"/>
       <c r="J624" s="11"/>
     </row>
     <row r="625" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B625" s="337"/>
-      <c r="C625" s="332" t="s">
-        <v>500</v>
-      </c>
-      <c r="D625" s="333"/>
-      <c r="E625" s="22" t="s">
-        <v>490</v>
-      </c>
-      <c r="F625" s="18">
-        <v>23</v>
-      </c>
-      <c r="G625" s="18">
-        <f>IFERROR(VLOOKUP(E625,AnswerCTBL,2,FALSE),0)</f>
-        <v>0.2</v>
-      </c>
-      <c r="H625" s="104"/>
-      <c r="I625" s="326"/>
+      <c r="C625" s="210" t="s">
+        <v>370</v>
+      </c>
+      <c r="D625" s="291" t="s">
+        <v>656</v>
+      </c>
+      <c r="E625" s="288"/>
+      <c r="F625" s="25"/>
+      <c r="G625" s="25"/>
+      <c r="H625" s="116"/>
+      <c r="I625" s="327"/>
       <c r="J625" s="11"/>
     </row>
     <row r="626" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B626" s="337"/>
-      <c r="C626" s="209" t="s">
-        <v>370</v>
-      </c>
-      <c r="D626" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E626" s="29"/>
-      <c r="F626" s="24"/>
-      <c r="G626" s="24"/>
-      <c r="H626" s="118"/>
-      <c r="I626" s="327"/>
+      <c r="C626" s="212"/>
+      <c r="D626" s="581"/>
+      <c r="E626" s="31"/>
+      <c r="F626" s="26"/>
+      <c r="G626" s="26"/>
+      <c r="H626" s="117"/>
+      <c r="I626" s="328"/>
       <c r="J626" s="11"/>
     </row>
     <row r="627" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B627" s="337"/>
-      <c r="C627" s="210" t="s">
-        <v>370</v>
-      </c>
-      <c r="D627" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E627" s="30"/>
-      <c r="F627" s="25"/>
-      <c r="G627" s="25"/>
-      <c r="H627" s="116"/>
-      <c r="I627" s="327"/>
+      <c r="C627" s="332" t="s">
+        <v>649</v>
+      </c>
+      <c r="D627" s="333"/>
+      <c r="E627" s="22" t="s">
+        <v>490</v>
+      </c>
+      <c r="F627" s="18">
+        <v>24</v>
+      </c>
+      <c r="G627" s="18">
+        <f>IFERROR(VLOOKUP(E627,AnswerCTBL,2,FALSE),0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H627" s="104"/>
+      <c r="I627" s="582"/>
       <c r="J627" s="11"/>
     </row>
     <row r="628" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B628" s="337"/>
-      <c r="C628" s="210" t="s">
+      <c r="C628" s="209" t="s">
         <v>370</v>
       </c>
       <c r="D628" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E628" s="30"/>
-      <c r="F628" s="25"/>
-      <c r="G628" s="25"/>
-      <c r="H628" s="116"/>
-      <c r="I628" s="327"/>
+        <v>657</v>
+      </c>
+      <c r="E628" s="29"/>
+      <c r="F628" s="24"/>
+      <c r="G628" s="24"/>
+      <c r="H628" s="118"/>
+      <c r="I628" s="397"/>
       <c r="J628" s="11"/>
     </row>
     <row r="629" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B629" s="338"/>
-      <c r="C629" s="212"/>
-      <c r="D629" s="21"/>
-      <c r="E629" s="31"/>
-      <c r="F629" s="26"/>
-      <c r="G629" s="26"/>
-      <c r="H629" s="117"/>
-      <c r="I629" s="328"/>
+      <c r="B629" s="337"/>
+      <c r="C629" s="210" t="s">
+        <v>370</v>
+      </c>
+      <c r="D629" s="291" t="s">
+        <v>658</v>
+      </c>
+      <c r="E629" s="288"/>
+      <c r="F629" s="25"/>
+      <c r="G629" s="25"/>
+      <c r="H629" s="116"/>
+      <c r="I629" s="397"/>
       <c r="J629" s="11"/>
     </row>
     <row r="630" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B630" s="339"/>
-      <c r="C630" s="340"/>
-      <c r="D630" s="340"/>
-      <c r="E630" s="340"/>
-      <c r="F630" s="340"/>
-      <c r="G630" s="340"/>
-      <c r="H630" s="340"/>
-      <c r="I630" s="341"/>
-      <c r="J630" s="11"/>
-    </row>
-    <row r="631" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B631" s="336" t="s">
-        <v>507</v>
-      </c>
-      <c r="C631" s="334" t="s">
-        <v>500</v>
-      </c>
-      <c r="D631" s="335"/>
-      <c r="E631" s="5" t="s">
+      <c r="B630" s="579"/>
+      <c r="C630" s="278" t="s">
+        <v>370</v>
+      </c>
+      <c r="D630" s="291" t="s">
+        <v>659</v>
+      </c>
+      <c r="E630" s="288"/>
+      <c r="F630" s="280"/>
+      <c r="G630" s="280"/>
+      <c r="H630" s="281"/>
+      <c r="I630" s="397"/>
+      <c r="J630" s="277"/>
+    </row>
+    <row r="631" spans="2:10" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B631" s="337"/>
+      <c r="C631" s="278" t="s">
+        <v>370</v>
+      </c>
+      <c r="D631" s="291" t="s">
+        <v>660</v>
+      </c>
+      <c r="E631" s="288"/>
+      <c r="F631" s="25"/>
+      <c r="G631" s="25"/>
+      <c r="H631" s="116"/>
+      <c r="I631" s="397"/>
+      <c r="J631" s="11"/>
+    </row>
+    <row r="632" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B632" s="579"/>
+      <c r="C632" s="278"/>
+      <c r="D632" s="291"/>
+      <c r="E632" s="288"/>
+      <c r="F632" s="280"/>
+      <c r="G632" s="280"/>
+      <c r="H632" s="281"/>
+      <c r="I632" s="397"/>
+      <c r="J632" s="277"/>
+    </row>
+    <row r="633" spans="2:10" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B633" s="579"/>
+      <c r="C633" s="583" t="s">
+        <v>650</v>
+      </c>
+      <c r="D633" s="584"/>
+      <c r="E633" s="282" t="s">
+        <v>490</v>
+      </c>
+      <c r="F633" s="283">
+        <v>25</v>
+      </c>
+      <c r="G633" s="283">
+        <f>IFERROR(VLOOKUP(E633,AnswerCTBL,2,FALSE),0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H633" s="284"/>
+      <c r="I633" s="585"/>
+      <c r="J633" s="277"/>
+    </row>
+    <row r="634" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B634" s="579"/>
+      <c r="C634" s="561" t="s">
+        <v>370</v>
+      </c>
+      <c r="D634" s="562" t="s">
+        <v>651</v>
+      </c>
+      <c r="E634" s="288"/>
+      <c r="F634" s="280"/>
+      <c r="G634" s="280"/>
+      <c r="H634" s="281"/>
+      <c r="I634" s="397"/>
+      <c r="J634" s="277"/>
+    </row>
+    <row r="635" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B635" s="579"/>
+      <c r="C635" s="278" t="s">
+        <v>370</v>
+      </c>
+      <c r="D635" s="291" t="s">
+        <v>652</v>
+      </c>
+      <c r="E635" s="288"/>
+      <c r="F635" s="280"/>
+      <c r="G635" s="280"/>
+      <c r="H635" s="281"/>
+      <c r="I635" s="397"/>
+      <c r="J635" s="277"/>
+    </row>
+    <row r="636" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B636" s="579"/>
+      <c r="C636" s="210" t="s">
+        <v>370</v>
+      </c>
+      <c r="D636" s="291" t="s">
+        <v>653</v>
+      </c>
+      <c r="E636" s="288"/>
+      <c r="F636" s="280"/>
+      <c r="G636" s="280"/>
+      <c r="H636" s="281"/>
+      <c r="I636" s="397"/>
+      <c r="J636" s="277"/>
+    </row>
+    <row r="637" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B637" s="579"/>
+      <c r="C637" s="210" t="s">
+        <v>370</v>
+      </c>
+      <c r="D637" s="291" t="s">
+        <v>661</v>
+      </c>
+      <c r="E637" s="288"/>
+      <c r="F637" s="280"/>
+      <c r="G637" s="280"/>
+      <c r="H637" s="281"/>
+      <c r="I637" s="397"/>
+      <c r="J637" s="277"/>
+    </row>
+    <row r="638" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B638" s="338"/>
+      <c r="C638" s="212"/>
+      <c r="D638" s="581"/>
+      <c r="E638" s="31"/>
+      <c r="F638" s="26"/>
+      <c r="G638" s="26"/>
+      <c r="H638" s="117"/>
+      <c r="I638" s="569"/>
+      <c r="J638" s="11"/>
+    </row>
+    <row r="639" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B639" s="339"/>
+      <c r="C639" s="340"/>
+      <c r="D639" s="340"/>
+      <c r="E639" s="340"/>
+      <c r="F639" s="340"/>
+      <c r="G639" s="340"/>
+      <c r="H639" s="340"/>
+      <c r="I639" s="341"/>
+      <c r="J639" s="11"/>
+    </row>
+    <row r="640" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B640" s="336" t="s">
+        <v>505</v>
+      </c>
+      <c r="C640" s="334" t="s">
+        <v>662</v>
+      </c>
+      <c r="D640" s="335"/>
+      <c r="E640" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="F631" s="18">
-        <v>24</v>
-      </c>
-      <c r="G631" s="18">
-        <f>IFERROR(VLOOKUP(E631,AnswerFTBL,2,FALSE),0)</f>
+      <c r="F640" s="18">
+        <v>26</v>
+      </c>
+      <c r="G640" s="18">
+        <f>IFERROR(VLOOKUP(E640,AnswerFTBL,2,FALSE),0)</f>
         <v>0.5</v>
       </c>
-      <c r="H631" s="104">
-        <f>IFERROR(AVERAGE(G631,G637),0)</f>
-        <v>0.35</v>
-      </c>
-      <c r="I631" s="326"/>
-      <c r="J631" s="11"/>
-    </row>
-    <row r="632" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B632" s="337"/>
-      <c r="C632" s="209" t="s">
-        <v>370</v>
-      </c>
-      <c r="D632" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E632" s="29"/>
-      <c r="F632" s="24"/>
-      <c r="G632" s="24"/>
-      <c r="H632" s="118"/>
-      <c r="I632" s="327"/>
-      <c r="J632" s="11"/>
-    </row>
-    <row r="633" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B633" s="337"/>
-      <c r="C633" s="210" t="s">
-        <v>370</v>
-      </c>
-      <c r="D633" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E633" s="30"/>
-      <c r="F633" s="25"/>
-      <c r="G633" s="25"/>
-      <c r="H633" s="116"/>
-      <c r="I633" s="327"/>
-      <c r="J633" s="11"/>
-    </row>
-    <row r="634" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B634" s="337"/>
-      <c r="C634" s="210" t="s">
-        <v>370</v>
-      </c>
-      <c r="D634" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E634" s="30"/>
-      <c r="F634" s="25"/>
-      <c r="G634" s="25"/>
-      <c r="H634" s="116"/>
-      <c r="I634" s="327"/>
-      <c r="J634" s="11"/>
-    </row>
-    <row r="635" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B635" s="337"/>
-      <c r="C635" s="210" t="s">
-        <v>370</v>
-      </c>
-      <c r="D635" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E635" s="30"/>
-      <c r="F635" s="25"/>
-      <c r="G635" s="25"/>
-      <c r="H635" s="116"/>
-      <c r="I635" s="327"/>
-      <c r="J635" s="11"/>
-    </row>
-    <row r="636" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B636" s="337"/>
-      <c r="C636" s="212"/>
-      <c r="D636" s="21"/>
-      <c r="E636" s="31"/>
-      <c r="F636" s="26"/>
-      <c r="G636" s="26"/>
-      <c r="H636" s="117"/>
-      <c r="I636" s="328"/>
-      <c r="J636" s="11"/>
-    </row>
-    <row r="637" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B637" s="337"/>
-      <c r="C637" s="332" t="s">
-        <v>500</v>
-      </c>
-      <c r="D637" s="333"/>
-      <c r="E637" s="22" t="s">
-        <v>425</v>
-      </c>
-      <c r="F637" s="18">
-        <v>25</v>
-      </c>
-      <c r="G637" s="18">
-        <f>IFERROR(VLOOKUP(E637,AnswerDTBL,2,FALSE),0)</f>
-        <v>0.2</v>
-      </c>
-      <c r="H637" s="104"/>
-      <c r="I637" s="326"/>
-      <c r="J637" s="11"/>
-    </row>
-    <row r="638" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B638" s="337"/>
-      <c r="C638" s="209" t="s">
-        <v>370</v>
-      </c>
-      <c r="D638" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E638" s="29"/>
-      <c r="F638" s="24"/>
-      <c r="G638" s="24"/>
-      <c r="H638" s="118"/>
-      <c r="I638" s="327"/>
-      <c r="J638" s="11"/>
-    </row>
-    <row r="639" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B639" s="337"/>
-      <c r="C639" s="210" t="s">
-        <v>370</v>
-      </c>
-      <c r="D639" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E639" s="30"/>
-      <c r="F639" s="25"/>
-      <c r="G639" s="25"/>
-      <c r="H639" s="116"/>
-      <c r="I639" s="327"/>
-      <c r="J639" s="11"/>
-    </row>
-    <row r="640" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B640" s="337"/>
-      <c r="C640" s="210" t="s">
-        <v>370</v>
-      </c>
-      <c r="D640" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E640" s="30"/>
-      <c r="F640" s="25"/>
-      <c r="G640" s="25"/>
-      <c r="H640" s="116"/>
-      <c r="I640" s="327"/>
+      <c r="H640" s="104">
+        <f>IFERROR(AVERAGE(G640,G644,G650,G654),0)</f>
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="I640" s="326"/>
       <c r="J640" s="11"/>
     </row>
     <row r="641" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B641" s="337"/>
-      <c r="C641" s="210" t="s">
+      <c r="C641" s="209" t="s">
         <v>370</v>
       </c>
       <c r="D641" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="E641" s="30"/>
-      <c r="F641" s="25"/>
-      <c r="G641" s="25"/>
-      <c r="H641" s="116"/>
+        <v>675</v>
+      </c>
+      <c r="E641" s="29"/>
+      <c r="F641" s="24"/>
+      <c r="G641" s="24"/>
+      <c r="H641" s="118"/>
       <c r="I641" s="327"/>
       <c r="J641" s="11"/>
     </row>
     <row r="642" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B642" s="338"/>
-      <c r="C642" s="212"/>
-      <c r="D642" s="21"/>
-      <c r="E642" s="31"/>
-      <c r="F642" s="26"/>
-      <c r="G642" s="26"/>
-      <c r="H642" s="117"/>
-      <c r="I642" s="328"/>
+      <c r="B642" s="337"/>
+      <c r="C642" s="210" t="s">
+        <v>370</v>
+      </c>
+      <c r="D642" s="291" t="s">
+        <v>676</v>
+      </c>
+      <c r="E642" s="288"/>
+      <c r="F642" s="25"/>
+      <c r="G642" s="25"/>
+      <c r="H642" s="116"/>
+      <c r="I642" s="327"/>
       <c r="J642" s="11"/>
+    </row>
+    <row r="643" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B643" s="337"/>
+      <c r="C643" s="212"/>
+      <c r="D643" s="21"/>
+      <c r="E643" s="31"/>
+      <c r="F643" s="26"/>
+      <c r="G643" s="26"/>
+      <c r="H643" s="117"/>
+      <c r="I643" s="328"/>
+      <c r="J643" s="11"/>
+    </row>
+    <row r="644" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B644" s="337"/>
+      <c r="C644" s="332" t="s">
+        <v>663</v>
+      </c>
+      <c r="D644" s="333"/>
+      <c r="E644" s="22" t="s">
+        <v>425</v>
+      </c>
+      <c r="F644" s="18">
+        <v>27</v>
+      </c>
+      <c r="G644" s="18">
+        <f>IFERROR(VLOOKUP(E644,AnswerDTBL,2,FALSE),0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H644" s="104"/>
+      <c r="I644" s="582"/>
+      <c r="J644" s="11"/>
+    </row>
+    <row r="645" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B645" s="337"/>
+      <c r="C645" s="209" t="s">
+        <v>370</v>
+      </c>
+      <c r="D645" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="E645" s="29"/>
+      <c r="F645" s="24"/>
+      <c r="G645" s="24"/>
+      <c r="H645" s="118"/>
+      <c r="I645" s="397"/>
+      <c r="J645" s="11"/>
+    </row>
+    <row r="646" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B646" s="337"/>
+      <c r="C646" s="210" t="s">
+        <v>370</v>
+      </c>
+      <c r="D646" s="291" t="s">
+        <v>672</v>
+      </c>
+      <c r="E646" s="288"/>
+      <c r="F646" s="25"/>
+      <c r="G646" s="25"/>
+      <c r="H646" s="116"/>
+      <c r="I646" s="397"/>
+      <c r="J646" s="11"/>
+    </row>
+    <row r="647" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B647" s="337"/>
+      <c r="C647" s="210" t="s">
+        <v>370</v>
+      </c>
+      <c r="D647" s="291" t="s">
+        <v>673</v>
+      </c>
+      <c r="E647" s="288"/>
+      <c r="F647" s="25"/>
+      <c r="G647" s="25"/>
+      <c r="H647" s="116"/>
+      <c r="I647" s="397"/>
+      <c r="J647" s="11"/>
+    </row>
+    <row r="648" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B648" s="579"/>
+      <c r="C648" s="278" t="s">
+        <v>370</v>
+      </c>
+      <c r="D648" s="291" t="s">
+        <v>674</v>
+      </c>
+      <c r="E648" s="288"/>
+      <c r="F648" s="280"/>
+      <c r="G648" s="280"/>
+      <c r="H648" s="281"/>
+      <c r="I648" s="397"/>
+      <c r="J648" s="277"/>
+    </row>
+    <row r="649" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B649" s="579"/>
+      <c r="C649" s="278"/>
+      <c r="D649" s="291"/>
+      <c r="E649" s="288"/>
+      <c r="F649" s="280"/>
+      <c r="G649" s="280"/>
+      <c r="H649" s="281"/>
+      <c r="I649" s="569"/>
+      <c r="J649" s="277"/>
+    </row>
+    <row r="650" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B650" s="579"/>
+      <c r="C650" s="575" t="s">
+        <v>665</v>
+      </c>
+      <c r="D650" s="576"/>
+      <c r="E650" s="586" t="s">
+        <v>425</v>
+      </c>
+      <c r="F650" s="283">
+        <v>28</v>
+      </c>
+      <c r="G650" s="283">
+        <f>IFERROR(VLOOKUP(E650,AnswerDTBL,2,FALSE),0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H650" s="284"/>
+      <c r="I650" s="582"/>
+      <c r="J650" s="277"/>
+    </row>
+    <row r="651" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B651" s="579"/>
+      <c r="C651" s="209" t="s">
+        <v>370</v>
+      </c>
+      <c r="D651" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="E651" s="288"/>
+      <c r="F651" s="280"/>
+      <c r="G651" s="280"/>
+      <c r="H651" s="281"/>
+      <c r="I651" s="397"/>
+      <c r="J651" s="277"/>
+    </row>
+    <row r="652" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B652" s="579"/>
+      <c r="C652" s="278" t="s">
+        <v>370</v>
+      </c>
+      <c r="D652" s="291" t="s">
+        <v>670</v>
+      </c>
+      <c r="E652" s="288"/>
+      <c r="F652" s="280"/>
+      <c r="G652" s="280"/>
+      <c r="H652" s="281"/>
+      <c r="I652" s="397"/>
+      <c r="J652" s="277"/>
+    </row>
+    <row r="653" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B653" s="579"/>
+      <c r="C653" s="278"/>
+      <c r="D653" s="291"/>
+      <c r="E653" s="288"/>
+      <c r="F653" s="280"/>
+      <c r="G653" s="280"/>
+      <c r="H653" s="281"/>
+      <c r="I653" s="569"/>
+      <c r="J653" s="277"/>
+    </row>
+    <row r="654" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B654" s="579"/>
+      <c r="C654" s="575" t="s">
+        <v>664</v>
+      </c>
+      <c r="D654" s="576"/>
+      <c r="E654" s="586" t="s">
+        <v>425</v>
+      </c>
+      <c r="F654" s="283">
+        <v>29</v>
+      </c>
+      <c r="G654" s="283">
+        <f>IFERROR(VLOOKUP(E654,AnswerDTBL,2,FALSE),0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="H654" s="284"/>
+      <c r="I654" s="582"/>
+      <c r="J654" s="277"/>
+    </row>
+    <row r="655" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B655" s="579"/>
+      <c r="C655" s="561" t="s">
+        <v>370</v>
+      </c>
+      <c r="D655" s="562" t="s">
+        <v>666</v>
+      </c>
+      <c r="E655" s="288"/>
+      <c r="F655" s="280"/>
+      <c r="G655" s="280"/>
+      <c r="H655" s="281"/>
+      <c r="I655" s="397"/>
+      <c r="J655" s="277"/>
+    </row>
+    <row r="656" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B656" s="579"/>
+      <c r="C656" s="278" t="s">
+        <v>370</v>
+      </c>
+      <c r="D656" s="291" t="s">
+        <v>667</v>
+      </c>
+      <c r="E656" s="288"/>
+      <c r="F656" s="280"/>
+      <c r="G656" s="280"/>
+      <c r="H656" s="281"/>
+      <c r="I656" s="397"/>
+      <c r="J656" s="277"/>
+    </row>
+    <row r="657" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B657" s="579"/>
+      <c r="C657" s="278" t="s">
+        <v>370</v>
+      </c>
+      <c r="D657" s="291" t="s">
+        <v>668</v>
+      </c>
+      <c r="E657" s="288"/>
+      <c r="F657" s="280"/>
+      <c r="G657" s="280"/>
+      <c r="H657" s="281"/>
+      <c r="I657" s="397"/>
+      <c r="J657" s="277"/>
+    </row>
+    <row r="658" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B658" s="579"/>
+      <c r="C658" s="278"/>
+      <c r="D658" s="291"/>
+      <c r="E658" s="288"/>
+      <c r="F658" s="280"/>
+      <c r="G658" s="280"/>
+      <c r="H658" s="281"/>
+      <c r="I658" s="397"/>
+      <c r="J658" s="277"/>
+    </row>
+    <row r="659" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B659" s="337"/>
+      <c r="C659" s="210"/>
+      <c r="D659" s="19"/>
+      <c r="E659" s="30"/>
+      <c r="F659" s="25"/>
+      <c r="G659" s="25"/>
+      <c r="H659" s="116"/>
+      <c r="I659" s="397"/>
+      <c r="J659" s="11"/>
+    </row>
+    <row r="660" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B660" s="338"/>
+      <c r="C660" s="212"/>
+      <c r="D660" s="21"/>
+      <c r="E660" s="31"/>
+      <c r="F660" s="26"/>
+      <c r="G660" s="26"/>
+      <c r="H660" s="117"/>
+      <c r="I660" s="569"/>
+      <c r="J660" s="11"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -37633,7 +38085,9 @@
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="349">
+  <mergeCells count="357">
+    <mergeCell ref="I650:I653"/>
+    <mergeCell ref="I654:I660"/>
     <mergeCell ref="C302:D302"/>
     <mergeCell ref="C307:D307"/>
     <mergeCell ref="C324:D324"/>
@@ -37648,21 +38102,27 @@
     <mergeCell ref="I328:I333"/>
     <mergeCell ref="I324:I327"/>
     <mergeCell ref="I318:I323"/>
-    <mergeCell ref="B630:I630"/>
-    <mergeCell ref="B631:B642"/>
-    <mergeCell ref="C631:D631"/>
-    <mergeCell ref="I631:I636"/>
-    <mergeCell ref="C637:D637"/>
-    <mergeCell ref="I637:I642"/>
-    <mergeCell ref="J607:J611"/>
-    <mergeCell ref="C612:D612"/>
-    <mergeCell ref="I612:I616"/>
-    <mergeCell ref="B617:I617"/>
-    <mergeCell ref="B618:B629"/>
-    <mergeCell ref="C618:D618"/>
-    <mergeCell ref="I618:I624"/>
-    <mergeCell ref="C625:D625"/>
-    <mergeCell ref="I625:I629"/>
+    <mergeCell ref="B639:I639"/>
+    <mergeCell ref="B640:B660"/>
+    <mergeCell ref="C640:D640"/>
+    <mergeCell ref="I640:I643"/>
+    <mergeCell ref="C644:D644"/>
+    <mergeCell ref="J607:J612"/>
+    <mergeCell ref="C613:D613"/>
+    <mergeCell ref="B621:I621"/>
+    <mergeCell ref="B622:B638"/>
+    <mergeCell ref="C622:D622"/>
+    <mergeCell ref="I622:I626"/>
+    <mergeCell ref="C627:D627"/>
+    <mergeCell ref="C617:D617"/>
+    <mergeCell ref="C633:D633"/>
+    <mergeCell ref="C650:D650"/>
+    <mergeCell ref="C654:D654"/>
+    <mergeCell ref="I627:I632"/>
+    <mergeCell ref="I633:I638"/>
+    <mergeCell ref="I617:I620"/>
+    <mergeCell ref="I613:I616"/>
+    <mergeCell ref="I644:I649"/>
     <mergeCell ref="B478:I478"/>
     <mergeCell ref="B479:B493"/>
     <mergeCell ref="C479:D479"/>
@@ -37670,9 +38130,9 @@
     <mergeCell ref="C486:D486"/>
     <mergeCell ref="I486:I493"/>
     <mergeCell ref="B606:D606"/>
-    <mergeCell ref="B607:B616"/>
+    <mergeCell ref="B607:B620"/>
     <mergeCell ref="C607:D607"/>
-    <mergeCell ref="I607:I611"/>
+    <mergeCell ref="I607:I612"/>
     <mergeCell ref="B494:J494"/>
     <mergeCell ref="C528:D528"/>
     <mergeCell ref="C550:D550"/>
@@ -37994,19 +38454,19 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E411 E356 M28:P28 M23:P23" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>AnswerB</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E191 E179 E203 E207 E214 E226 E233 E237 E252 E195 E336 E344 E351 E362 E378 E388 E401 E406 E421 E426 E522 E528 E540 E550 E569 E575 E582 E589 E185 E118 E111 E41 E89 E35 E48 E105 E534 E417 E270 E81 E23 E28 E44 E62 E199 E496 E504 E518 E157 E153 E142 E297 E292 E285 E473 E454 E438 E625 E618 E612 E443 E486 E479 E147 E161 E302 E307 E448" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E191 E179 E203 E207 E214 E226 E233 E237 E252 E195 E336 E344 E351 E362 E378 E388 E401 E406 E421 E426 E522 E528 E540 E550 E569 E575 E582 E589 E185 E118 E111 E41 E89 E35 E48 E105 E534 E417 E270 E81 E23 E28 E44 E62 E199 E496 E504 E518 E157 E153 E142 E297 E292 E285 E473 E454 E438 E627 E622 E613 E443 E486 E479 E147 E161 E302 E307 E448 E617 E633" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>AnswerC</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E18 E500 M18:P18" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>AnswerA</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E56 E240 E130 E100 E274 E597 E169 E137 E318 E279 E637 E607 E173 E324 E328" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E56 E240 E130 E100 E274 E597 E169 E137 E318 E279 E644 E607 E173 E324 E328 E650 E654" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>AnswerD</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E65 E601 E462" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>AnswerE</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E73 E124 E247 E264 E220 E558 E367 E396 E429 E384 E166 E314 E434 E631" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E73 E124 E247 E264 E220 E558 E367 E396 E429 E384 E166 E314 E434 E640" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>AnswerF</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E257 E562 E508 E374 E545 E393 E94" xr:uid="{00000000-0002-0000-0100-000006000000}">
@@ -38541,7 +39001,7 @@
       </c>
       <c r="J17" s="102">
         <f>AVERAGE(C26:C29)</f>
-        <v>1.0499999999999998</v>
+        <v>1.03125</v>
       </c>
       <c r="L17" s="221"/>
       <c r="M17" s="221"/>
@@ -38730,7 +39190,7 @@
         <v>149</v>
       </c>
       <c r="B21" s="79" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C21" s="102">
         <f>Interview!$J$279</f>
@@ -38760,7 +39220,7 @@
         <v>149</v>
       </c>
       <c r="U21" s="79" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="V21" s="102">
         <v>0</v>
@@ -38943,7 +39403,7 @@
         <v>222</v>
       </c>
       <c r="B25" s="84" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C25" s="102">
         <f>Interview!$J$434</f>
@@ -38973,7 +39433,7 @@
         <v>222</v>
       </c>
       <c r="U25" s="84" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="V25" s="102">
         <v>0</v>
@@ -39156,23 +39616,23 @@
         <v>373</v>
       </c>
       <c r="B29" s="89" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C29" s="102">
         <f>Interview!$J$607</f>
-        <v>0.75</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="D29" s="102">
         <f>Interview!H607</f>
-        <v>0.2</v>
+        <v>0.20000000000000004</v>
       </c>
       <c r="E29" s="102">
-        <f>Interview!H618</f>
-        <v>0.2</v>
+        <f>Interview!H622</f>
+        <v>0.20000000000000004</v>
       </c>
       <c r="F29" s="102">
-        <f>Interview!H631</f>
-        <v>0.35</v>
+        <f>Interview!H640</f>
+        <v>0.27499999999999997</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -39186,7 +39646,7 @@
         <v>373</v>
       </c>
       <c r="U29" s="89" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="V29" s="102">
         <v>0</v>
@@ -39199,7 +39659,7 @@
       </c>
       <c r="Y29" s="102">
         <f>Interview!$J$607</f>
-        <v>0.75</v>
+        <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -39788,7 +40248,7 @@
         <v>149</v>
       </c>
       <c r="B46" s="79" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C46" s="102">
         <f>Roadmap!Y87</f>
@@ -39821,7 +40281,7 @@
         <v>149</v>
       </c>
       <c r="U46" s="79" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="V46" s="102">
         <v>0</v>
@@ -40004,7 +40464,7 @@
         <v>222</v>
       </c>
       <c r="B50" s="84" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C50" s="102">
         <f>Roadmap!Y125</f>
@@ -40037,7 +40497,7 @@
         <v>222</v>
       </c>
       <c r="U50" s="84" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="V50" s="102">
         <v>0</v>
@@ -40211,7 +40671,7 @@
         <v>373</v>
       </c>
       <c r="B54" s="89" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C54" s="102">
         <f>Roadmap!Y165</f>
@@ -40241,7 +40701,7 @@
         <v>373</v>
       </c>
       <c r="U54" s="89" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="V54" s="102">
         <v>0</v>
@@ -44172,7 +44632,7 @@
         <v>15</v>
       </c>
       <c r="B49" s="465" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C49" s="427" t="str">
         <f>Interview!C137</f>
@@ -44340,7 +44800,7 @@
         <v>17</v>
       </c>
       <c r="B52" s="465" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C52" s="427" t="str">
         <f>Interview!C153</f>
@@ -44491,7 +44951,7 @@
         <v>19</v>
       </c>
       <c r="B55" s="465" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C55" s="427" t="str">
         <f>Interview!C166</f>
@@ -46107,7 +46567,7 @@
     </row>
     <row r="86" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B86" s="458" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C86" s="459"/>
       <c r="D86" s="502"/>
@@ -46156,7 +46616,7 @@
         <v>15</v>
       </c>
       <c r="B87" s="451" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C87" s="427" t="str">
         <f>Interview!C279</f>
@@ -46326,7 +46786,7 @@
         <v>17</v>
       </c>
       <c r="B90" s="451" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C90" s="427" t="str">
         <f>Interview!C292</f>
@@ -46483,7 +46943,7 @@
         <v>19</v>
       </c>
       <c r="B93" s="451" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C93" s="427" t="str">
         <f>Interview!C314</f>
@@ -48107,7 +48567,7 @@
     </row>
     <row r="124" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B124" s="503" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C124" s="504"/>
       <c r="D124" s="512"/>
@@ -48156,7 +48616,7 @@
         <v>15</v>
       </c>
       <c r="B125" s="447" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C125" s="427" t="str">
         <f>Interview!C434</f>
@@ -48304,7 +48764,7 @@
       </c>
       <c r="B127" s="448"/>
       <c r="C127" s="429" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D127" s="430"/>
       <c r="E127" s="30" t="str">
@@ -48388,7 +48848,7 @@
         <v>17</v>
       </c>
       <c r="B129" s="529" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C129" s="427" t="str">
         <f>Interview!C454</f>
@@ -48523,7 +48983,7 @@
     <row r="131" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B131" s="531"/>
       <c r="C131" s="429" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D131" s="430"/>
       <c r="E131" s="30" t="str">
@@ -48605,7 +49065,7 @@
         <v>19</v>
       </c>
       <c r="B133" s="447" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C133" s="427" t="str">
         <f>Interview!C479</f>
@@ -50243,7 +50703,7 @@
     </row>
     <row r="164" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B164" s="434" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C164" s="435"/>
       <c r="D164" s="436"/>
@@ -50292,11 +50752,11 @@
         <v>15</v>
       </c>
       <c r="B165" s="425" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C165" s="427" t="str">
         <f>Interview!C607</f>
-        <v>___?</v>
+        <v>Does your organization gather information about new vulnerability issues?</v>
       </c>
       <c r="D165" s="428"/>
       <c r="E165" s="30" t="str">
@@ -50381,12 +50841,12 @@
       </c>
       <c r="B166" s="426"/>
       <c r="C166" s="429" t="str">
-        <f>Interview!C612</f>
-        <v>___?</v>
+        <f>Interview!C613</f>
+        <v>Are vulnerability issues filtered to dedicated project, used hardware and software stacks?</v>
       </c>
       <c r="D166" s="430"/>
       <c r="E166" s="30" t="str">
-        <f>Interview!E612</f>
+        <f>Interview!E613</f>
         <v>Yes, a small percentage are/do</v>
       </c>
       <c r="F166" s="18">
@@ -50460,15 +50920,15 @@
         <v>17</v>
       </c>
       <c r="B168" s="425" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C168" s="427" t="str">
-        <f>Interview!C618</f>
-        <v>___?</v>
+        <f>Interview!C622</f>
+        <v>Is your penetration test continuously developed?</v>
       </c>
       <c r="D168" s="428"/>
       <c r="E168" s="30" t="str">
-        <f>Interview!E618</f>
+        <f>Interview!E622</f>
         <v>Yes, a small percentage are/do</v>
       </c>
       <c r="F168" s="147">
@@ -50532,12 +50992,12 @@
       </c>
       <c r="B169" s="426"/>
       <c r="C169" s="429" t="str">
-        <f>Interview!C625</f>
-        <v>___?</v>
+        <f>Interview!C627</f>
+        <v>Do you assure that penetration tests are executed for every released hardware/software combination?</v>
       </c>
       <c r="D169" s="430"/>
       <c r="E169" s="30" t="str">
-        <f>Interview!E625</f>
+        <f>Interview!E627</f>
         <v>Yes, a small percentage are/do</v>
       </c>
       <c r="F169" s="18">
@@ -50611,15 +51071,15 @@
         <v>19</v>
       </c>
       <c r="B171" s="425" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C171" s="427" t="str">
-        <f>Interview!C631</f>
-        <v>___?</v>
+        <f>Interview!C640</f>
+        <v>Does your company know how to contact the end users of your devices?</v>
       </c>
       <c r="D171" s="428"/>
       <c r="E171" s="30" t="str">
-        <f>Interview!E631</f>
+        <f>Interview!E640</f>
         <v>Yes, there is a standard set</v>
       </c>
       <c r="F171" s="147">
@@ -50683,12 +51143,12 @@
       </c>
       <c r="B172" s="431"/>
       <c r="C172" s="432" t="str">
-        <f>Interview!C637</f>
-        <v>___?</v>
+        <f>Interview!C644</f>
+        <v>Does your company have a process which defines the propagation of security vulnerabilities to your customers?</v>
       </c>
       <c r="D172" s="433"/>
       <c r="E172" s="30" t="str">
-        <f>Interview!E637</f>
+        <f>Interview!E644</f>
         <v>Yes, we did it once</v>
       </c>
       <c r="F172" s="18">
@@ -52020,7 +52480,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A19" s="96" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B19" s="105">
         <f>IF(ISNUMBER(Interview!$J$279),Interview!$J$279,SUM(LEFT(Interview!$J$279),".5"))</f>
@@ -52345,7 +52805,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A23" s="94" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B23" s="105">
         <f>IF(ISNUMBER(Interview!$J$434),Interview!$J$434,SUM(LEFT(Interview!$J$434),".5"))</f>
@@ -52673,11 +53133,11 @@
     </row>
     <row r="27" spans="1:31" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="92" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B27" s="243">
         <f>IF(ISNUMBER(Interview!$J$607),Interview!$J$607,SUM(LEFT(Interview!$J$607),".5"))</f>
-        <v>0.75</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="C27" s="199">
         <f>Roadmap!M165</f>
@@ -52710,7 +53170,7 @@
       <c r="J27" s="51"/>
       <c r="K27" s="248">
         <f t="shared" si="0"/>
-        <v>-0.65</v>
+        <v>-0.57500000000000007</v>
       </c>
       <c r="L27" s="206"/>
       <c r="M27" s="206"/>
@@ -52747,7 +53207,7 @@
       </c>
       <c r="AE27" s="128">
         <f t="shared" si="6"/>
-        <v>0.75</v>
+        <v>0.67500000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.15">
@@ -52781,7 +53241,7 @@
       </c>
       <c r="C29" s="128">
         <f>SUM(C12:C27)-SUM(B12:B27)</f>
-        <v>-8.3583333333333343</v>
+        <v>-8.283333333333335</v>
       </c>
       <c r="D29" s="128"/>
       <c r="E29" s="128">
@@ -52801,7 +53261,7 @@
       <c r="J29" s="128"/>
       <c r="K29" s="248">
         <f>SUM(K12:K27)</f>
-        <v>-8.7583333333333329</v>
+        <v>-8.6833333333333318</v>
       </c>
       <c r="L29" s="206"/>
       <c r="M29" s="206"/>
@@ -52821,23 +53281,23 @@
       <c r="B30" s="52"/>
       <c r="C30" s="53">
         <f>C29/$K$29</f>
-        <v>0.95432921027592787</v>
+        <v>0.95393474088291785</v>
       </c>
       <c r="E30" s="53">
         <f>E29/$K$29</f>
-        <v>0.35394862036156038</v>
+        <v>0.35700575815738966</v>
       </c>
       <c r="G30" s="53">
         <f>G29/$K$29</f>
-        <v>0.14272121788772604</v>
+        <v>0.143953934740883</v>
       </c>
       <c r="I30" s="53">
         <f>I29/$K$29</f>
-        <v>-0.45099904852521405</v>
+        <v>-0.45489443378119004</v>
       </c>
       <c r="K30" s="250">
         <f>1-K29/24</f>
-        <v>1.3649305555555555</v>
+        <v>1.3618055555555555</v>
       </c>
       <c r="L30" s="206"/>
       <c r="M30" s="206"/>

</xml_diff>